<commit_message>
Cleaned up to removed unused code and files. Improved annotations and knitted all markdown files.
</commit_message>
<xml_diff>
--- a/data/Supplementary_Table_1.xlsx
+++ b/data/Supplementary_Table_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Terkild\Documents\Git\CITE-seq_optimization\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Terkild2\Documents\Git\CITE-seq_optimization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D905AE1-00CA-4814-98E3-3EA5B9DDC477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C792AA5-19AD-4643-880B-DDA6B23E1AAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6860D6EA-EBA9-4F68-9E7B-4C39ECF5C4FA}"/>
+    <workbookView xWindow="5745" yWindow="2025" windowWidth="15465" windowHeight="11385" xr2:uid="{6860D6EA-EBA9-4F68-9E7B-4C39ECF5C4FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="218">
   <si>
     <t>Marker</t>
   </si>
@@ -669,6 +669,24 @@
   </si>
   <si>
     <t>IgG2A</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -724,7 +742,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
@@ -747,10 +784,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D0129EE-038D-4CE6-8668-7A1D0C86F646}" name="Tabel1" displayName="Tabel1" ref="A1:J53" totalsRowShown="0">
-  <autoFilter ref="A1:J53" xr:uid="{1418F33D-218B-4175-B683-473AD244AF26}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8A5FFC90-ED4F-495A-BD0F-88EC87A27115}" name="Marker" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D0129EE-038D-4CE6-8668-7A1D0C86F646}" name="Tabel1" displayName="Tabel1" ref="A1:K53" totalsRowShown="0">
+  <autoFilter ref="A1:K53" xr:uid="{1418F33D-218B-4175-B683-473AD244AF26}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K53">
+    <sortCondition ref="A1:A53"/>
+  </sortState>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{8A5FFC90-ED4F-495A-BD0F-88EC87A27115}" name="Marker" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{547D3A63-4345-4370-A3C2-AC66949A13F7}" name="Category" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{BB84F0DC-1F67-46BD-99AA-212B1EFAD291}" name="Alias"/>
     <tableColumn id="3" xr3:uid="{96D8D38D-FBAD-4E26-9548-67915622D95C}" name="Clone"/>
     <tableColumn id="4" xr3:uid="{8D0A57D4-3386-4DED-9112-2A9C37DE8E97}" name="Isotype_Mouse"/>
@@ -758,9 +799,9 @@
     <tableColumn id="6" xr3:uid="{620E5F8B-7A92-4C29-851F-B0D3B1FFACFF}" name="TotalSeqC_Tag"/>
     <tableColumn id="7" xr3:uid="{0B9F323F-DECB-41DB-A08A-057F36FA00DA}" name="BioLegend_Cat"/>
     <tableColumn id="8" xr3:uid="{F0A90913-E323-4AC8-893A-3E163CF8F656}" name="Stock_conc_µg_per_mL"/>
-    <tableColumn id="9" xr3:uid="{4DD7B326-F17C-46AF-A5D4-B9C1D4A46675}" name="conc_µg_per_mL" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{4DD7B326-F17C-46AF-A5D4-B9C1D4A46675}" name="conc_µg_per_mL" dataDxfId="1"/>
     <tableColumn id="10" xr3:uid="{A8EEB628-35B3-4A6E-81E3-E8BD5187F4A4}" name="dilution_1x">
-      <calculatedColumnFormula>H2/I2</calculatedColumnFormula>
+      <calculatedColumnFormula>I2/J2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1064,1649 +1105,1808 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DBDE5C-9031-4576-ADBD-F0164FE6652E}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="1" max="2" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>205</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>204</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>206</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>207</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>208</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>209</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>350233</v>
       </c>
-      <c r="H2">
-        <v>500</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="I2">
+        <v>500</v>
+      </c>
+      <c r="J2" s="1">
         <v>1.25</v>
       </c>
-      <c r="J2">
-        <f>H2/I2</f>
+      <c r="K2">
+        <f>I2/J2</f>
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>328649</v>
       </c>
-      <c r="H3">
-        <v>500</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="I3">
+        <v>500</v>
+      </c>
+      <c r="J3" s="1">
         <v>2.5</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J53" si="0">H3/I3</f>
+      <c r="K3">
+        <f>I3/J3</f>
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
       <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>16</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>313243</v>
       </c>
-      <c r="H4">
-        <v>500</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="I4">
+        <v>500</v>
+      </c>
+      <c r="J4" s="1">
         <v>2.5</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
+      <c r="K4">
+        <f>I4/J4</f>
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
       <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>301359</v>
       </c>
-      <c r="H5">
-        <v>500</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="I5">
+        <v>500</v>
+      </c>
+      <c r="J5" s="1">
         <v>0.625</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
+      <c r="K5">
+        <f>I5/J5</f>
         <v>800</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
       <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>306045</v>
       </c>
-      <c r="H6">
-        <v>500</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="I6">
+        <v>500</v>
+      </c>
+      <c r="J6" s="1">
         <v>0.5</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
+      <c r="K6">
+        <f>I6/J6</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
       <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>29</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>351356</v>
       </c>
-      <c r="H7">
-        <v>500</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="I7">
+        <v>500</v>
+      </c>
+      <c r="J7" s="1">
         <v>1.25</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
+      <c r="K7">
+        <f>I7/J7</f>
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
       <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
         <v>33</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>34</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>350035</v>
       </c>
-      <c r="H8">
-        <v>500</v>
-      </c>
-      <c r="I8" s="1">
-        <v>5</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
+      <c r="I8">
+        <v>500</v>
+      </c>
+      <c r="J8" s="1">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <f>I8/J8</f>
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
       <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
         <v>37</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>38</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>352327</v>
       </c>
-      <c r="H9">
-        <v>500</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="I9">
+        <v>500</v>
+      </c>
+      <c r="J9" s="1">
         <v>3</v>
       </c>
-      <c r="J9" s="2">
-        <f t="shared" si="0"/>
+      <c r="K9" s="2">
+        <f>I9/J9</f>
         <v>166.66666666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D10" t="s">
         <v>40</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>41</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>39</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>42</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>301859</v>
       </c>
-      <c r="H10">
-        <v>500</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="I10">
+        <v>500</v>
+      </c>
+      <c r="J10" s="1">
         <v>1</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <f>I10/J10</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>45</v>
       </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
       <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
         <v>46</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>47</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>344125</v>
       </c>
-      <c r="H11">
-        <v>500</v>
-      </c>
-      <c r="I11" s="1">
+      <c r="I11">
+        <v>500</v>
+      </c>
+      <c r="J11" s="1">
         <v>1.25</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
+      <c r="K11">
+        <f>I11/J11</f>
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C12" t="s">
         <v>49</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>41</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>49</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>51</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>369621</v>
       </c>
-      <c r="H12">
-        <v>500</v>
-      </c>
-      <c r="I12" s="1">
+      <c r="I12">
+        <v>500</v>
+      </c>
+      <c r="J12" s="1">
         <v>10</v>
       </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
+      <c r="K12">
+        <f>I12/J12</f>
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C13" t="s">
         <v>53</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>54</v>
       </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
       <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
         <v>53</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>55</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>353747</v>
       </c>
-      <c r="H13">
-        <v>500</v>
-      </c>
-      <c r="I13" s="1">
+      <c r="I13">
+        <v>500</v>
+      </c>
+      <c r="J13" s="1">
         <v>10</v>
       </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
+      <c r="K13">
+        <f>I13/J13</f>
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B14" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D14" t="s">
         <v>57</v>
       </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
       <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
         <v>56</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>58</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>302265</v>
       </c>
-      <c r="H14">
-        <v>500</v>
-      </c>
-      <c r="I14" s="1">
+      <c r="I14">
+        <v>500</v>
+      </c>
+      <c r="J14" s="1">
         <v>1</v>
       </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <f>I14/J14</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" t="s">
         <v>60</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>61</v>
       </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
       <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
         <v>60</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>62</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>359425</v>
       </c>
-      <c r="H15">
-        <v>500</v>
-      </c>
-      <c r="I15" s="1">
+      <c r="I15">
+        <v>500</v>
+      </c>
+      <c r="J15" s="1">
         <v>1.25</v>
       </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
+      <c r="K15">
+        <f>I15/J15</f>
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" t="s">
         <v>64</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>65</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>66</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>64</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>67</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>353440</v>
       </c>
-      <c r="H16">
-        <v>500</v>
-      </c>
-      <c r="I16" s="1">
+      <c r="I16">
+        <v>500</v>
+      </c>
+      <c r="J16" s="1">
         <v>0.625</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
+      <c r="K16">
+        <f>I16/J16</f>
         <v>800</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C17" t="s">
         <v>69</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>70</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>41</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>69</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>71</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>353251</v>
       </c>
-      <c r="H17">
-        <v>500</v>
-      </c>
-      <c r="I17" s="1">
+      <c r="I17">
+        <v>500</v>
+      </c>
+      <c r="J17" s="1">
         <v>10</v>
       </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
+      <c r="K17">
+        <f>I17/J17</f>
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B18" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D18" t="s">
         <v>73</v>
       </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
       <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
         <v>74</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>75</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>300135</v>
       </c>
-      <c r="H18">
-        <v>500</v>
-      </c>
-      <c r="I18" s="1">
-        <v>5</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="0"/>
+      <c r="I18">
+        <v>500</v>
+      </c>
+      <c r="J18" s="1">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <f>I18/J18</f>
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C19" t="s">
+      <c r="B19" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D19" t="s">
         <v>77</v>
       </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
       <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
         <v>78</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>79</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>331547</v>
       </c>
-      <c r="H19">
-        <v>500</v>
-      </c>
-      <c r="I19" s="1">
+      <c r="I19">
+        <v>500</v>
+      </c>
+      <c r="J19" s="1">
         <v>0.5</v>
       </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
+      <c r="K19">
+        <f>I19/J19</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C20" t="s">
+      <c r="B20" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D20" t="s">
         <v>81</v>
       </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
       <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
         <v>80</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>82</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>309231</v>
       </c>
-      <c r="H20">
-        <v>500</v>
-      </c>
-      <c r="I20" s="1">
+      <c r="I20">
+        <v>500</v>
+      </c>
+      <c r="J20" s="1">
         <v>0.1</v>
       </c>
-      <c r="J20">
-        <f t="shared" si="0"/>
+      <c r="K20">
+        <f>I20/J20</f>
         <v>5000</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B21" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D21" t="s">
         <v>84</v>
       </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
       <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
         <v>85</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>86</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>369335</v>
       </c>
-      <c r="H21">
-        <v>500</v>
-      </c>
-      <c r="I21" s="1">
+      <c r="I21">
+        <v>500</v>
+      </c>
+      <c r="J21" s="1">
         <v>1</v>
       </c>
-      <c r="J21">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f>I21/J21</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B22" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D22" t="s">
         <v>88</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>41</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>87</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>89</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>311143</v>
       </c>
-      <c r="H22">
-        <v>500</v>
-      </c>
-      <c r="I22" s="1">
+      <c r="I22">
+        <v>500</v>
+      </c>
+      <c r="J22" s="1">
         <v>3.3000000000000007</v>
       </c>
-      <c r="J22" s="2">
-        <f t="shared" si="0"/>
+      <c r="K22" s="2">
+        <f>I22/J22</f>
         <v>151.51515151515147</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C23" t="s">
+      <c r="B23" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D23" t="s">
         <v>91</v>
       </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
       <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
         <v>92</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>93</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>302649</v>
       </c>
-      <c r="H23">
-        <v>500</v>
-      </c>
-      <c r="I23" s="1">
+      <c r="I23">
+        <v>500</v>
+      </c>
+      <c r="J23" s="1">
         <v>1.25</v>
       </c>
-      <c r="J23">
-        <f t="shared" si="0"/>
+      <c r="K23">
+        <f>I23/J23</f>
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C24" t="s">
         <v>95</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>96</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>41</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>95</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>97</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>302722</v>
       </c>
-      <c r="H24">
-        <v>500</v>
-      </c>
-      <c r="I24" s="1">
+      <c r="I24">
+        <v>500</v>
+      </c>
+      <c r="J24" s="1">
         <v>1.25</v>
       </c>
-      <c r="J24">
-        <f t="shared" si="0"/>
+      <c r="K24">
+        <f>I24/J24</f>
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C25" t="s">
         <v>99</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>100</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>41</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>98</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>101</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>329751</v>
       </c>
-      <c r="H25">
-        <v>500</v>
-      </c>
-      <c r="I25" s="1">
+      <c r="I25">
+        <v>500</v>
+      </c>
+      <c r="J25" s="1">
         <v>1.25</v>
       </c>
-      <c r="J25">
-        <f t="shared" si="0"/>
+      <c r="K25">
+        <f>I25/J25</f>
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C26" t="s">
         <v>103</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>104</v>
       </c>
-      <c r="D26" t="s">
-        <v>5</v>
-      </c>
       <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
         <v>105</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>106</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>329963</v>
       </c>
-      <c r="H26">
-        <v>500</v>
-      </c>
-      <c r="I26" s="1">
-        <v>5</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="0"/>
+      <c r="I26">
+        <v>500</v>
+      </c>
+      <c r="J26" s="1">
+        <v>5</v>
+      </c>
+      <c r="K26">
+        <f>I26/J26</f>
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C27" t="s">
+      <c r="B27" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D27" t="s">
         <v>108</v>
       </c>
-      <c r="D27" t="s">
-        <v>5</v>
-      </c>
       <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" t="s">
         <v>107</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>109</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>302963</v>
       </c>
-      <c r="H27">
-        <v>500</v>
-      </c>
-      <c r="I27" s="1">
+      <c r="I27">
+        <v>500</v>
+      </c>
+      <c r="J27" s="1">
         <v>1.25</v>
       </c>
-      <c r="J27">
-        <f t="shared" si="0"/>
+      <c r="K27">
+        <f>I27/J27</f>
         <v>400</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C28" t="s">
+      <c r="B28" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D28" t="s">
         <v>111</v>
       </c>
-      <c r="D28" t="s">
-        <v>5</v>
-      </c>
       <c r="E28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" t="s">
         <v>112</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>113</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>300479</v>
       </c>
-      <c r="H28">
-        <v>500</v>
-      </c>
-      <c r="I28" s="1">
+      <c r="I28">
+        <v>500</v>
+      </c>
+      <c r="J28" s="1">
         <v>0.5</v>
       </c>
-      <c r="J28">
-        <f t="shared" si="0"/>
+      <c r="K28">
+        <f>I28/J28</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C29" t="s">
+      <c r="B29" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D29" t="s">
         <v>115</v>
       </c>
-      <c r="D29" t="s">
-        <v>5</v>
-      </c>
       <c r="E29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
         <v>116</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>117</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>333919</v>
       </c>
-      <c r="H29">
-        <v>500</v>
-      </c>
-      <c r="I29" s="1">
-        <v>5</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="0"/>
+      <c r="I29">
+        <v>500</v>
+      </c>
+      <c r="J29" s="1">
+        <v>5</v>
+      </c>
+      <c r="K29">
+        <f>I29/J29</f>
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" t="s">
         <v>119</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>120</v>
       </c>
-      <c r="D30" t="s">
-        <v>5</v>
-      </c>
       <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
         <v>121</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>122</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>303139</v>
       </c>
-      <c r="H30">
-        <v>500</v>
-      </c>
-      <c r="I30" s="1">
+      <c r="I30">
+        <v>500</v>
+      </c>
+      <c r="J30" s="1">
         <v>0.1</v>
       </c>
-      <c r="J30">
-        <f t="shared" si="0"/>
+      <c r="K30">
+        <f>I30/J30</f>
         <v>5000</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C31" t="s">
+      <c r="B31" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D31" t="s">
         <v>124</v>
       </c>
-      <c r="D31" t="s">
-        <v>5</v>
-      </c>
       <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" t="s">
         <v>125</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>126</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>345049</v>
       </c>
-      <c r="H31">
-        <v>500</v>
-      </c>
-      <c r="I31" s="1">
+      <c r="I31">
+        <v>500</v>
+      </c>
+      <c r="J31" s="1">
         <v>2.5</v>
       </c>
-      <c r="J31">
-        <f t="shared" si="0"/>
+      <c r="K31">
+        <f>I31/J31</f>
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B32" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D32" t="s">
         <v>128</v>
       </c>
-      <c r="D32" t="s">
-        <v>5</v>
-      </c>
       <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
         <v>129</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>130</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>328237</v>
       </c>
-      <c r="H32">
-        <v>500</v>
-      </c>
-      <c r="I32" s="1">
+      <c r="I32">
+        <v>500</v>
+      </c>
+      <c r="J32" s="1">
         <v>0.625</v>
       </c>
-      <c r="J32">
-        <f t="shared" si="0"/>
+      <c r="K32">
+        <f>I32/J32</f>
         <v>800</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C33" t="s">
+      <c r="B33" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D33" t="s">
         <v>132</v>
       </c>
-      <c r="D33" t="s">
-        <v>5</v>
-      </c>
       <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" t="s">
         <v>131</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>133</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>300567</v>
       </c>
-      <c r="H33">
-        <v>500</v>
-      </c>
-      <c r="I33" s="1">
+      <c r="I33">
+        <v>500</v>
+      </c>
+      <c r="J33" s="1">
         <v>1</v>
       </c>
-      <c r="J33">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <f>I33/J33</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C34" t="s">
+      <c r="B34" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D34" t="s">
         <v>135</v>
       </c>
-      <c r="D34" t="s">
-        <v>5</v>
-      </c>
       <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" t="s">
         <v>134</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>136</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>338827</v>
       </c>
-      <c r="H34">
-        <v>500</v>
-      </c>
-      <c r="I34" s="1">
+      <c r="I34">
+        <v>500</v>
+      </c>
+      <c r="J34" s="1">
         <v>5.000000000000001E-2</v>
       </c>
-      <c r="J34">
-        <f t="shared" si="0"/>
+      <c r="K34">
+        <f>I34/J34</f>
         <v>9999.9999999999982</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C35" t="s">
+      <c r="B35" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D35" t="s">
         <v>138</v>
       </c>
-      <c r="D35" t="s">
-        <v>5</v>
-      </c>
       <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" t="s">
         <v>139</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>140</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>304068</v>
       </c>
-      <c r="H35">
-        <v>500</v>
-      </c>
-      <c r="I35" s="1">
+      <c r="I35">
+        <v>500</v>
+      </c>
+      <c r="J35" s="1">
         <v>0.1</v>
       </c>
-      <c r="J35">
-        <f t="shared" si="0"/>
+      <c r="K35">
+        <f>I35/J35</f>
         <v>5000</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C36" t="s">
+      <c r="B36" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D36" t="s">
         <v>142</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>66</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>139</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>143</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>304163</v>
       </c>
-      <c r="H36">
-        <v>500</v>
-      </c>
-      <c r="I36" s="1">
+      <c r="I36">
+        <v>500</v>
+      </c>
+      <c r="J36" s="1">
         <v>0.625</v>
       </c>
-      <c r="J36">
-        <f t="shared" si="0"/>
+      <c r="K36">
+        <f>I36/J36</f>
         <v>800</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C37" t="s">
+      <c r="B37" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D37" t="s">
         <v>145</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>41</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>139</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>146</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>304259</v>
       </c>
-      <c r="H37">
-        <v>500</v>
-      </c>
-      <c r="I37" s="1">
+      <c r="I37">
+        <v>500</v>
+      </c>
+      <c r="J37" s="1">
         <v>1.25</v>
       </c>
-      <c r="J37">
-        <f t="shared" si="0"/>
+      <c r="K37">
+        <f>I37/J37</f>
         <v>400</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C38" t="s">
+      <c r="B38" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D38" t="s">
         <v>148</v>
       </c>
-      <c r="D38" t="s">
-        <v>5</v>
-      </c>
       <c r="E38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" t="s">
         <v>147</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>149</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>300637</v>
       </c>
-      <c r="H38">
-        <v>500</v>
-      </c>
-      <c r="I38" s="1">
+      <c r="I38">
+        <v>500</v>
+      </c>
+      <c r="J38" s="1">
         <v>0.625</v>
       </c>
-      <c r="J38">
-        <f t="shared" si="0"/>
+      <c r="K38">
+        <f>I38/J38</f>
         <v>800</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C39" t="s">
+      <c r="B39" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D39" t="s">
         <v>151</v>
       </c>
-      <c r="D39" t="s">
-        <v>5</v>
-      </c>
       <c r="E39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" t="s">
         <v>152</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>153</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>362559</v>
       </c>
-      <c r="H39">
-        <v>500</v>
-      </c>
-      <c r="I39" s="1">
+      <c r="I39">
+        <v>500</v>
+      </c>
+      <c r="J39" s="1">
         <v>1</v>
       </c>
-      <c r="J39">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <f>I39/J39</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C40" t="s">
+      <c r="B40" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D40" t="s">
         <v>155</v>
       </c>
-      <c r="D40" t="s">
-        <v>5</v>
-      </c>
       <c r="E40" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" t="s">
         <v>156</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>157</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>304851</v>
       </c>
-      <c r="H40">
-        <v>500</v>
-      </c>
-      <c r="I40" s="1">
+      <c r="I40">
+        <v>500</v>
+      </c>
+      <c r="J40" s="1">
         <v>1.25</v>
       </c>
-      <c r="J40">
-        <f t="shared" si="0"/>
+      <c r="K40">
+        <f>I40/J40</f>
         <v>400</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C41" t="s">
+      <c r="B41" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D41" t="s">
         <v>159</v>
       </c>
-      <c r="D41" t="s">
-        <v>5</v>
-      </c>
       <c r="E41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" t="s">
         <v>160</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>161</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>392909</v>
       </c>
-      <c r="H41">
-        <v>500</v>
-      </c>
-      <c r="I41" s="1">
+      <c r="I41">
+        <v>500</v>
+      </c>
+      <c r="J41" s="1">
         <v>1</v>
       </c>
-      <c r="J41">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <f>I41/J41</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C42" t="s">
+      <c r="B42" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D42" t="s">
         <v>163</v>
       </c>
-      <c r="D42" t="s">
-        <v>5</v>
-      </c>
       <c r="E42" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" t="s">
         <v>162</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>164</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>310951</v>
       </c>
-      <c r="H42">
-        <v>500</v>
-      </c>
-      <c r="I42" s="1">
+      <c r="I42">
+        <v>500</v>
+      </c>
+      <c r="J42" s="1">
         <v>0.625</v>
       </c>
-      <c r="J42">
-        <f t="shared" si="0"/>
+      <c r="K42">
+        <f>I42/J42</f>
         <v>800</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C43" t="s">
+      <c r="B43" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D43" t="s">
         <v>166</v>
       </c>
-      <c r="D43" t="s">
-        <v>5</v>
-      </c>
       <c r="E43" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43" t="s">
         <v>165</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>167</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>355119</v>
       </c>
-      <c r="H43">
-        <v>500</v>
-      </c>
-      <c r="I43" s="1">
+      <c r="I43">
+        <v>500</v>
+      </c>
+      <c r="J43" s="1">
         <v>0.625</v>
       </c>
-      <c r="J43">
-        <f t="shared" si="0"/>
+      <c r="K43">
+        <f>I43/J43</f>
         <v>800</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C44" t="s">
+      <c r="B44" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D44" t="s">
         <v>169</v>
       </c>
-      <c r="D44" t="s">
-        <v>5</v>
-      </c>
       <c r="E44" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44" t="s">
         <v>170</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>171</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>301071</v>
       </c>
-      <c r="H44">
-        <v>500</v>
-      </c>
-      <c r="I44" s="1">
+      <c r="I44">
+        <v>500</v>
+      </c>
+      <c r="J44" s="1">
         <v>0.625</v>
       </c>
-      <c r="J44">
-        <f t="shared" si="0"/>
+      <c r="K44">
+        <f>I44/J44</f>
         <v>800</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C45" t="s">
         <v>173</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>174</v>
       </c>
-      <c r="D45" t="s">
-        <v>5</v>
-      </c>
       <c r="E45" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" t="s">
         <v>172</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>175</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>305243</v>
       </c>
-      <c r="H45">
-        <v>500</v>
-      </c>
-      <c r="I45" s="1">
+      <c r="I45">
+        <v>500</v>
+      </c>
+      <c r="J45" s="1">
         <v>1.25</v>
       </c>
-      <c r="J45">
-        <f t="shared" si="0"/>
+      <c r="K45">
+        <f>I45/J45</f>
         <v>400</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C46" t="s">
         <v>177</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>178</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>66</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>176</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>179</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>305447</v>
       </c>
-      <c r="H46">
-        <v>500</v>
-      </c>
-      <c r="I46" s="1">
+      <c r="I46">
+        <v>500</v>
+      </c>
+      <c r="J46" s="1">
         <v>10</v>
       </c>
-      <c r="J46">
-        <f t="shared" si="0"/>
+      <c r="K46">
+        <f>I46/J46</f>
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C47" t="s">
+      <c r="B47" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D47" t="s">
         <v>181</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>66</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>182</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>183</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>324247</v>
       </c>
-      <c r="H47">
-        <v>500</v>
-      </c>
-      <c r="I47" s="1">
+      <c r="I47">
+        <v>500</v>
+      </c>
+      <c r="J47" s="1">
         <v>0.625</v>
       </c>
-      <c r="J47">
-        <f t="shared" si="0"/>
+      <c r="K47">
+        <f>I47/J47</f>
         <v>800</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C48" t="s">
+      <c r="B48" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D48" t="s">
         <v>185</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>41</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>186</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>187</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>311449</v>
       </c>
-      <c r="H48">
-        <v>500</v>
-      </c>
-      <c r="I48" s="1">
+      <c r="I48">
+        <v>500</v>
+      </c>
+      <c r="J48" s="1">
         <v>1</v>
       </c>
-      <c r="J48">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <f>I48/J48</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C49" t="s">
+      <c r="B49" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D49" t="s">
         <v>189</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>41</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>190</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>191</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>307663</v>
       </c>
-      <c r="H49">
-        <v>500</v>
-      </c>
-      <c r="I49" s="1">
+      <c r="I49">
+        <v>500</v>
+      </c>
+      <c r="J49" s="1">
         <v>1.6500000000000004</v>
       </c>
-      <c r="J49" s="2">
-        <f t="shared" si="0"/>
+      <c r="K49" s="2">
+        <f>I49/J49</f>
         <v>303.03030303030295</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C50" t="s">
+      <c r="B50" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D50" t="s">
         <v>192</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>193</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>400187</v>
       </c>
-      <c r="H50">
-        <v>500</v>
-      </c>
-      <c r="I50" s="1">
+      <c r="I50">
+        <v>500</v>
+      </c>
+      <c r="J50" s="1">
         <v>2.5</v>
       </c>
-      <c r="J50">
-        <f t="shared" si="0"/>
+      <c r="K50">
+        <f>I50/J50</f>
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C51" t="s">
+      <c r="B51" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D51" t="s">
         <v>194</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>195</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>400293</v>
       </c>
-      <c r="H51">
-        <v>500</v>
-      </c>
-      <c r="I51" s="1">
+      <c r="I51">
+        <v>500</v>
+      </c>
+      <c r="J51" s="1">
         <v>2.5</v>
       </c>
-      <c r="J51">
-        <f t="shared" si="0"/>
+      <c r="K51">
+        <f>I51/J51</f>
         <v>200</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C52" t="s">
+      <c r="B52" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D52" t="s">
         <v>197</v>
       </c>
-      <c r="D52" t="s">
-        <v>5</v>
-      </c>
       <c r="E52" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" t="s">
         <v>198</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>199</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>306743</v>
       </c>
-      <c r="H52">
-        <v>500</v>
-      </c>
-      <c r="I52" s="1">
+      <c r="I52">
+        <v>500</v>
+      </c>
+      <c r="J52" s="1">
         <v>1.25</v>
       </c>
-      <c r="J52">
-        <f t="shared" si="0"/>
+      <c r="K52">
+        <f>I52/J52</f>
         <v>400</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C53" t="s">
+      <c r="B53" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D53" t="s">
         <v>201</v>
       </c>
-      <c r="D53" t="s">
-        <v>5</v>
-      </c>
       <c r="E53" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" t="s">
         <v>202</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>203</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>331231</v>
       </c>
-      <c r="H53">
-        <v>500</v>
-      </c>
-      <c r="I53" s="1">
+      <c r="I53">
+        <v>500</v>
+      </c>
+      <c r="J53" s="1">
         <v>10</v>
       </c>
-      <c r="J53">
-        <f t="shared" si="0"/>
+      <c r="K53">
+        <f>I53/J53</f>
         <v>50</v>
       </c>
     </row>

</xml_diff>